<commit_message>
añadimos tabla para gráficos
</commit_message>
<xml_diff>
--- a/Scripts/Results/Results/metrics_Prune_results.xlsx
+++ b/Scripts/Results/Results/metrics_Prune_results.xlsx
@@ -558,7 +558,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>689226dd329525e5bdc8847496b93ed862815da7dcb2d30f17f185f6469f69c2</t>
+          <t>36534d24ac281c0af20238b10f16af70370015b3c501b6401469c6885071ba6f</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -577,31 +577,31 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.9102827357447481</v>
+        <v>0.8882325067129996</v>
       </c>
       <c r="G3" t="n">
-        <v>0.04884953463110041</v>
+        <v>0.03627289360636618</v>
       </c>
       <c r="H3" t="n">
-        <v>0.8372401592215833</v>
+        <v>0.8385670057496682</v>
       </c>
       <c r="I3" t="n">
-        <v>0.02924074486405104</v>
+        <v>0.01850245861724849</v>
       </c>
       <c r="J3" t="n">
-        <v>0.8502358490566038</v>
+        <v>0.8508254716981132</v>
       </c>
       <c r="K3" t="n">
-        <v>0.004714181186918031</v>
+        <v>0.005208908520199198</v>
       </c>
       <c r="L3" t="n">
         <v>11223</v>
       </c>
       <c r="M3" t="n">
-        <v>6094</v>
+        <v>7818</v>
       </c>
       <c r="N3" t="n">
-        <v>1189.967447757721</v>
+        <v>1219.153937339783</v>
       </c>
     </row>
     <row r="4">
@@ -610,7 +610,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>6feadd50b9a6b076e54c2991e65f0e85c621fb5086c567f1f4f10d2a812cb1d4</t>
+          <t>2ac7da93cd63e2bac5f5c5165d6b01eac7280485147f271b2f3de11fcd463301</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -629,31 +629,31 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.9024482704154162</v>
+        <v>0.9080082135523614</v>
       </c>
       <c r="G4" t="n">
-        <v>0.07430079490065981</v>
+        <v>0.08194768214086647</v>
       </c>
       <c r="H4" t="n">
-        <v>0.8360607400855079</v>
+        <v>0.835765885301489</v>
       </c>
       <c r="I4" t="n">
-        <v>0.01162288368639666</v>
+        <v>0.02127974188131047</v>
       </c>
       <c r="J4" t="n">
-        <v>0.8449292452830188</v>
+        <v>0.8443396226415094</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0001765883051921963</v>
+        <v>2.238482165143815e-05</v>
       </c>
       <c r="L4" t="n">
         <v>11223</v>
       </c>
       <c r="M4" t="n">
-        <v>6796</v>
+        <v>6290</v>
       </c>
       <c r="N4" t="n">
-        <v>1037.828794717789</v>
+        <v>1387.968171834946</v>
       </c>
     </row>
     <row r="5">
@@ -662,7 +662,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>6e26d3ae4c496cd80e2feb6878f2e5aba35baf830bfe1ad03568276b53d7055d</t>
+          <t>e5ef36041274255de56088ecc2aaea4578b1d8a73afc3127b5dce4d11a6f9ea4</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -681,31 +681,31 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.8922761017216869</v>
+        <v>0.8863686621386827</v>
       </c>
       <c r="G5" t="n">
-        <v>0.06141927868121281</v>
+        <v>0.04425826046269848</v>
       </c>
       <c r="H5" t="n">
-        <v>0.8348813209494325</v>
+        <v>0.8390092879256966</v>
       </c>
       <c r="I5" t="n">
-        <v>0.02208672798424328</v>
+        <v>0.01261879835281288</v>
       </c>
       <c r="J5" t="n">
-        <v>0.8406544811320755</v>
+        <v>0.8419811320754716</v>
       </c>
       <c r="K5" t="n">
-        <v>4.504488439315696e-06</v>
+        <v>0.0001763349472987744</v>
       </c>
       <c r="L5" t="n">
         <v>11223</v>
       </c>
       <c r="M5" t="n">
-        <v>7268</v>
+        <v>7852</v>
       </c>
       <c r="N5" t="n">
-        <v>2756.312183856964</v>
+        <v>2616.466651678085</v>
       </c>
     </row>
     <row r="6">
@@ -766,7 +766,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>e774dc5fe82ad306f0ef9b8b2524260673b6d3383243402736ba9b9c6dca047c</t>
+          <t>acdfa119a061b04bf9c831fe40428cc5df5aab728f3d4dbad4126556c21de348</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -785,31 +785,31 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0.9464539567208972</v>
+        <v>0.9470857684410046</v>
       </c>
       <c r="G7" t="n">
-        <v>0.03042668143263944</v>
+        <v>0.03219150374810718</v>
       </c>
       <c r="H7" t="n">
-        <v>0.8314904909332154</v>
+        <v>0.8313430635412059</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0529486303907786</v>
+        <v>0.04519085247924348</v>
       </c>
       <c r="J7" t="n">
-        <v>0.8413915094339622</v>
+        <v>0.8394752358490566</v>
       </c>
       <c r="K7" t="n">
-        <v>0.0001895027259677939</v>
+        <v>0.0001922012461561332</v>
       </c>
       <c r="L7" t="n">
         <v>11223</v>
       </c>
       <c r="M7" t="n">
-        <v>3134</v>
+        <v>3076</v>
       </c>
       <c r="N7" t="n">
-        <v>1092.975595474243</v>
+        <v>1084.799773931503</v>
       </c>
     </row>
     <row r="8">
@@ -818,7 +818,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>31459fe6a0611114dd2dd74b1d76f9bd993d384e6860f50dbfdd7fcbd0f0f407</t>
+          <t>37a957d3d873c13324534781c6368b56c593938ab846a1e2cf576d052b82ae91</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -837,31 +837,31 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0.9581424735428842</v>
+        <v>0.9512557257937134</v>
       </c>
       <c r="G8" t="n">
-        <v>0.05512598957870559</v>
+        <v>0.03056370849534771</v>
       </c>
       <c r="H8" t="n">
-        <v>0.8279522335249889</v>
+        <v>0.8292790800530738</v>
       </c>
       <c r="I8" t="n">
-        <v>0.04701088109365299</v>
+        <v>0.0472828486835165</v>
       </c>
       <c r="J8" t="n">
-        <v>0.8377063679245284</v>
+        <v>0.8341686320754716</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0001380612978953352</v>
+        <v>7.341973911814681e-05</v>
       </c>
       <c r="L8" t="n">
         <v>11223</v>
       </c>
       <c r="M8" t="n">
-        <v>1940</v>
+        <v>2576</v>
       </c>
       <c r="N8" t="n">
-        <v>2615.874733686447</v>
+        <v>2301.582619428635</v>
       </c>
     </row>
     <row r="9">
@@ -870,7 +870,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>f71f327d336008fa23b62b48d1f1c90219e7a13422dc823291974949a02bb1c2</t>
+          <t>e869dd161023f5b8370aa76e060d10732606f78107d90c2eb0e568f102f4a2a9</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -889,31 +889,31 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>0.9498341494234718</v>
+        <v>0.961111988627389</v>
       </c>
       <c r="G9" t="n">
-        <v>0.04315909445479739</v>
+        <v>0.04760145338021594</v>
       </c>
       <c r="H9" t="n">
-        <v>0.8341441839893853</v>
+        <v>0.8273625239569512</v>
       </c>
       <c r="I9" t="n">
-        <v>0.04275762387314865</v>
+        <v>0.04910639817816283</v>
       </c>
       <c r="J9" t="n">
-        <v>0.8380011792452831</v>
+        <v>0.8365271226415094</v>
       </c>
       <c r="K9" t="n">
-        <v>0.0001120966694386216</v>
+        <v>3.19920927211656e-05</v>
       </c>
       <c r="L9" t="n">
         <v>11223</v>
       </c>
       <c r="M9" t="n">
-        <v>2686</v>
+        <v>1672</v>
       </c>
       <c r="N9" t="n">
-        <v>5950.334803104401</v>
+        <v>6102.205889463425</v>
       </c>
     </row>
     <row r="10">
@@ -974,7 +974,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>adce565c033838a59c9e85079060bb5096e9adecbdd592df0077ba508ee86ddd</t>
+          <t>5a5acdbc0e16338ce85de636eb79f50709bb0db54dbd219f37b803861123fe8b</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -993,31 +993,31 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>0.6842857142857143</v>
+        <v>0.7628571428571429</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>0.06576328013131696</v>
       </c>
       <c r="H11" t="n">
-        <v>0.7533333333333333</v>
+        <v>0.66</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>0.1879618226600986</v>
       </c>
       <c r="J11" t="n">
-        <v>0.72</v>
+        <v>0.74</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>0.02944843081829382</v>
       </c>
       <c r="L11" t="n">
         <v>293</v>
       </c>
       <c r="M11" t="n">
-        <v>292</v>
+        <v>218</v>
       </c>
       <c r="N11" t="n">
-        <v>0.0500030517578125</v>
+        <v>2.962201356887817</v>
       </c>
     </row>
     <row r="12">
@@ -1069,7 +1069,7 @@
         <v>292</v>
       </c>
       <c r="N12" t="n">
-        <v>60.744624376297</v>
+        <v>71.71288394927979</v>
       </c>
     </row>
     <row r="13">
@@ -1078,7 +1078,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>adce565c033838a59c9e85079060bb5096e9adecbdd592df0077ba508ee86ddd</t>
+          <t>4f6fc85550fea5e275b3e9a89d042434affa910e8a1bdd9a9e923f160de7fc12</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1118,10 +1118,10 @@
         <v>293</v>
       </c>
       <c r="M13" t="n">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N13" t="n">
-        <v>29.81589770317078</v>
+        <v>101.1658039093018</v>
       </c>
     </row>
     <row r="14">
@@ -1225,7 +1225,7 @@
         <v>292</v>
       </c>
       <c r="N15" t="n">
-        <v>0.1572906970977783</v>
+        <v>0.1889121532440186</v>
       </c>
     </row>
     <row r="16">
@@ -1277,7 +1277,7 @@
         <v>292</v>
       </c>
       <c r="N16" t="n">
-        <v>20.09589385986328</v>
+        <v>7.010198354721069</v>
       </c>
     </row>
     <row r="17">
@@ -1286,7 +1286,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>4f6fc85550fea5e275b3e9a89d042434affa910e8a1bdd9a9e923f160de7fc12</t>
+          <t>adce565c033838a59c9e85079060bb5096e9adecbdd592df0077ba508ee86ddd</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1326,10 +1326,10 @@
         <v>293</v>
       </c>
       <c r="M17" t="n">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="N17" t="n">
-        <v>102.2958285808563</v>
+        <v>6.323291063308716</v>
       </c>
     </row>
     <row r="18">
@@ -1390,7 +1390,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>f792ab3273a6a86e71c5c5852e73e2d9b04d69943fe3db98be60cdbed2452949</t>
+          <t>ca006ef6a3714cd02de31b9fed77382818273e69d36489631691435ddc0c0c76</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1409,31 +1409,31 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>0.8505560704355886</v>
+        <v>0.8549582947173309</v>
       </c>
       <c r="G19" t="n">
-        <v>0.03259123579581165</v>
+        <v>0.02301678074882059</v>
       </c>
       <c r="H19" t="n">
-        <v>0.64</v>
+        <v>0.6594594594594595</v>
       </c>
       <c r="I19" t="n">
-        <v>0.101281750788384</v>
+        <v>0.1321201746435256</v>
       </c>
       <c r="J19" t="n">
         <v>0.6857451403887689</v>
       </c>
       <c r="K19" t="n">
-        <v>0.0003328329515741857</v>
+        <v>0.0007825115910482794</v>
       </c>
       <c r="L19" t="n">
         <v>3055</v>
       </c>
       <c r="M19" t="n">
-        <v>1232</v>
+        <v>1330</v>
       </c>
       <c r="N19" t="n">
-        <v>87.33568549156189</v>
+        <v>88.56655550003052</v>
       </c>
     </row>
     <row r="20">
@@ -1442,7 +1442,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>944c0b7a053971e084f0c575d51d3232b15963ff6eea67c041faef5302aeec47</t>
+          <t>2b7b21ebd87769ed04c4c94047f99b507af9658347f32bb6097f7e3f43e649f2</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1461,31 +1461,31 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>0.8498609823911029</v>
+        <v>0.8470806302131604</v>
       </c>
       <c r="G20" t="n">
-        <v>0.01931640738034889</v>
+        <v>0.01393711274043437</v>
       </c>
       <c r="H20" t="n">
-        <v>0.6443243243243243</v>
+        <v>0.654054054054054</v>
       </c>
       <c r="I20" t="n">
-        <v>0.1300204613561997</v>
+        <v>0.1103918339141947</v>
       </c>
       <c r="J20" t="n">
-        <v>0.67170626349892</v>
+        <v>0.6727861771058316</v>
       </c>
       <c r="K20" t="n">
-        <v>0.001066625561338075</v>
+        <v>0.0009880461547140396</v>
       </c>
       <c r="L20" t="n">
         <v>3055</v>
       </c>
       <c r="M20" t="n">
-        <v>1436</v>
+        <v>1372</v>
       </c>
       <c r="N20" t="n">
-        <v>1093.945598602295</v>
+        <v>1495.69330573082</v>
       </c>
     </row>
     <row r="21">
@@ -1494,7 +1494,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>44e3ce013b966d2bab00a919c30459862c6f40bc355f3291867081da862f6fb9</t>
+          <t>8b99bc2fd7c9ddf5424d2a954b489643b81faf1f54f1168ab132011cd6f022a8</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1513,31 +1513,31 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>0.8410565338276181</v>
+        <v>0.8639944392956441</v>
       </c>
       <c r="G21" t="n">
-        <v>0.02327662069539001</v>
+        <v>0.02349019188051611</v>
       </c>
       <c r="H21" t="n">
-        <v>0.6454054054054054</v>
+        <v>0.6508108108108108</v>
       </c>
       <c r="I21" t="n">
-        <v>0.1378061172294803</v>
+        <v>0.1468731056746645</v>
       </c>
       <c r="J21" t="n">
-        <v>0.6576673866090713</v>
+        <v>0.6609071274298056</v>
       </c>
       <c r="K21" t="n">
-        <v>0.0009558643006088996</v>
+        <v>0.0008501577744506328</v>
       </c>
       <c r="L21" t="n">
         <v>3055</v>
       </c>
       <c r="M21" t="n">
-        <v>1462</v>
+        <v>1312</v>
       </c>
       <c r="N21" t="n">
-        <v>1813.240329265594</v>
+        <v>1858.950346231461</v>
       </c>
     </row>
     <row r="22">
@@ -1598,7 +1598,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>172588f19fc6c2cfb1b374cca1e8a722fc4d2e1f84627c4bfd7737cc147ee2ca</t>
+          <t>a3849443631f50710ef903503aa5eb84f838f98fda3b4e444bf8946278da788f</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1617,31 +1617,31 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>0.8241427247451344</v>
+        <v>0.8846153846153846</v>
       </c>
       <c r="G23" t="n">
-        <v>0.01682444841304195</v>
+        <v>0.02065451727642915</v>
       </c>
       <c r="H23" t="n">
-        <v>0.6767567567567567</v>
+        <v>0.6475675675675676</v>
       </c>
       <c r="I23" t="n">
-        <v>0.03559406037622531</v>
+        <v>0.05940247550255831</v>
       </c>
       <c r="J23" t="n">
-        <v>0.6803455723542117</v>
+        <v>0.6695464362850972</v>
       </c>
       <c r="K23" t="n">
-        <v>0.00144300144300144</v>
+        <v>0.001059704184704191</v>
       </c>
       <c r="L23" t="n">
         <v>3055</v>
       </c>
       <c r="M23" t="n">
-        <v>1538</v>
+        <v>846</v>
       </c>
       <c r="N23" t="n">
-        <v>89.89445328712463</v>
+        <v>83.73716354370117</v>
       </c>
     </row>
     <row r="24">
@@ -1650,7 +1650,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>fca8666827ae69362864e09ca625b751e36a88c22ce9fad930335c83f278b2d2</t>
+          <t>9a09243941d174a7a00c5414f9d59008da962b96fb9be6eb2ba8b1e1c3b01c7a</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1669,31 +1669,31 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>0.852873030583874</v>
+        <v>0.8677015755329008</v>
       </c>
       <c r="G24" t="n">
-        <v>0.01358408665878341</v>
+        <v>0.01456722315823222</v>
       </c>
       <c r="H24" t="n">
-        <v>0.6486486486486487</v>
+        <v>0.6572972972972972</v>
       </c>
       <c r="I24" t="n">
-        <v>0.04706728738540217</v>
+        <v>0.06360705195462565</v>
       </c>
       <c r="J24" t="n">
-        <v>0.6468682505399568</v>
+        <v>0.652267818574514</v>
       </c>
       <c r="K24" t="n">
-        <v>0.0008793290043290214</v>
+        <v>0.0005862193362193291</v>
       </c>
       <c r="L24" t="n">
         <v>3055</v>
       </c>
       <c r="M24" t="n">
-        <v>1242</v>
+        <v>1050</v>
       </c>
       <c r="N24" t="n">
-        <v>1308.248546123505</v>
+        <v>944.9122035503387</v>
       </c>
     </row>
     <row r="25">
@@ -1702,7 +1702,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4b600ec8bebf38d37e62a13eaeb1eaea884eb7f09a496f0e011be22c0e545374</t>
+          <t>1ba145b3ab8c051cc5fb26e73808437a66edb99285461b89d877b000bee2e333</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1721,31 +1721,31 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>0.8651529193697869</v>
+        <v>0.8653846153846154</v>
       </c>
       <c r="G25" t="n">
-        <v>0.02655363595288263</v>
+        <v>0.01596210333463903</v>
       </c>
       <c r="H25" t="n">
-        <v>0.6562162162162162</v>
+        <v>0.6518918918918919</v>
       </c>
       <c r="I25" t="n">
-        <v>0.06746287870001499</v>
+        <v>0.0473094863696315</v>
       </c>
       <c r="J25" t="n">
-        <v>0.6479481641468683</v>
+        <v>0.652267818574514</v>
       </c>
       <c r="K25" t="n">
-        <v>9.018759018764033e-05</v>
+        <v>0.0005862193362193291</v>
       </c>
       <c r="L25" t="n">
         <v>3055</v>
       </c>
       <c r="M25" t="n">
-        <v>1086</v>
+        <v>1032</v>
       </c>
       <c r="N25" t="n">
-        <v>2129.157821416855</v>
+        <v>2157.673085212708</v>
       </c>
     </row>
     <row r="26">
@@ -1806,7 +1806,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>b3725fac501957ea9235a8c02b3722d336db2a9262a9f89ed4e556e9d80b0219</t>
+          <t>cfaf7c0d29122cc6cb32d4011174aa2b41693be193403ea5f79cc1b16f20c7e7</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1825,31 +1825,31 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>0.9746028770910454</v>
+        <v>0.9671992877559628</v>
       </c>
       <c r="G27" t="n">
-        <v>0.02779587305095476</v>
+        <v>0.007810607827250043</v>
       </c>
       <c r="H27" t="n">
-        <v>0.8921933085501859</v>
+        <v>0.896348130330199</v>
       </c>
       <c r="I27" t="n">
-        <v>0.1283694766742547</v>
+        <v>0.1135450126719549</v>
       </c>
       <c r="J27" t="n">
-        <v>0.8959335373852209</v>
+        <v>0.8976825535636205</v>
       </c>
       <c r="K27" t="n">
-        <v>0.01073526380138954</v>
+        <v>0.01013418109993013</v>
       </c>
       <c r="L27" t="n">
         <v>3669</v>
       </c>
       <c r="M27" t="n">
-        <v>1272</v>
+        <v>1548</v>
       </c>
       <c r="N27" t="n">
-        <v>124.2718124389648</v>
+        <v>126.5933237075806</v>
       </c>
     </row>
     <row r="28">
@@ -1858,7 +1858,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>681135e189d388b0378c1f683dd70f44fa374393fe1025e04cab38c57f60d2c1</t>
+          <t>d67d2a96045fa1ed09d01938015ec7134e9fe8da2c491177f98787d2ef4af439</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1877,31 +1877,31 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>0.9530012651703295</v>
+        <v>0.9397404057916686</v>
       </c>
       <c r="G28" t="n">
-        <v>0.006758372267692249</v>
+        <v>0.005223628884854518</v>
       </c>
       <c r="H28" t="n">
-        <v>0.8941613820249289</v>
+        <v>0.9024710255849552</v>
       </c>
       <c r="I28" t="n">
-        <v>0.1056399622521327</v>
+        <v>0.08174070253590099</v>
       </c>
       <c r="J28" t="n">
-        <v>0.8893747267162221</v>
+        <v>0.8891560996939222</v>
       </c>
       <c r="K28" t="n">
-        <v>0.006271326012452141</v>
+        <v>0.007498373906090993</v>
       </c>
       <c r="L28" t="n">
         <v>3669</v>
       </c>
       <c r="M28" t="n">
-        <v>1974</v>
+        <v>2584</v>
       </c>
       <c r="N28" t="n">
-        <v>2645.492490768433</v>
+        <v>1707.465686321259</v>
       </c>
     </row>
     <row r="29">
@@ -1910,7 +1910,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>842ef93786b1044882995efe6bcc3c0469fe11adcdf5abcd1afa63f129c959dd</t>
+          <t>1306a25bff19959c6122e2e440e471fad920b2707c173f81a100b4b307f0ac2a</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1929,31 +1929,31 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>0.954172719179045</v>
+        <v>0.9658872592662012</v>
       </c>
       <c r="G29" t="n">
-        <v>0.01320377361675496</v>
+        <v>0.006935675895159401</v>
       </c>
       <c r="H29" t="n">
-        <v>0.8915372840586049</v>
+        <v>0.8987535534659961</v>
       </c>
       <c r="I29" t="n">
-        <v>0.1046614489588272</v>
+        <v>0.09568631081913033</v>
       </c>
       <c r="J29" t="n">
-        <v>0.8869698294709226</v>
+        <v>0.8856580673371228</v>
       </c>
       <c r="K29" t="n">
-        <v>0.0004980017263456517</v>
+        <v>0.0007716396998725533</v>
       </c>
       <c r="L29" t="n">
         <v>3669</v>
       </c>
       <c r="M29" t="n">
-        <v>1892</v>
+        <v>1560</v>
       </c>
       <c r="N29" t="n">
-        <v>3478.149893760681</v>
+        <v>2743.400072097778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>